<commit_message>
thiet ke man hinh -2
</commit_message>
<xml_diff>
--- a/03.Design/Shokai.xlsx
+++ b/03.Design/Shokai.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="Shokai" sheetId="1" r:id="rId1"/>
+    <sheet name="Top" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="3" r:id="rId2"/>
-    <sheet name="Shinki" sheetId="4" r:id="rId3"/>
+    <sheet name="Registration" sheetId="4" r:id="rId3"/>
     <sheet name="Edit" sheetId="5" r:id="rId4"/>
     <sheet name="Error1" sheetId="6" r:id="rId5"/>
     <sheet name="Error2" sheetId="7" r:id="rId6"/>
     <sheet name="Reminder" sheetId="8" r:id="rId7"/>
+    <sheet name="Registration_info" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>List item</t>
   </si>
@@ -249,6 +250,12 @@
   </si>
   <si>
     <t>2. Hiện thông báo sai form email</t>
+  </si>
+  <si>
+    <t>1. Button tiếp tục sử dụng</t>
+  </si>
+  <si>
+    <t>1. Sau khi chạm vào mục 2 thì chuyển sang màn hình mypage</t>
   </si>
 </sst>
 </file>
@@ -382,16 +389,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -406,7 +413,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3295650" y="4057650"/>
+          <a:off x="885825" y="3829050"/>
           <a:ext cx="323850" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -447,15 +454,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -470,7 +477,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3324225" y="4867275"/>
+          <a:off x="2867025" y="3876675"/>
           <a:ext cx="323850" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -510,16 +517,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -534,7 +541,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3324225" y="5648325"/>
+          <a:off x="1914525" y="5391150"/>
           <a:ext cx="323850" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1956,15 +1963,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1979,7 +1986,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124200" y="3419475"/>
+          <a:off x="3267075" y="3571875"/>
           <a:ext cx="323850" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2623,6 +2630,125 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>3</a:t>
+          </a:r>
+          <a:endParaRPr lang="vi-VN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8EDA7D5-5806-42E9-8844-BE3A0F6DA31D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="257175"/>
+          <a:ext cx="3571875" cy="6353175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B40A96-A30C-49CD-9E55-F0083B39B860}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3267075" y="5905500"/>
+          <a:ext cx="323850" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1</a:t>
           </a:r>
           <a:endParaRPr lang="vi-VN" sz="1100"/>
         </a:p>
@@ -2933,8 +3059,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3293,8 +3419,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18:K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3669,8 +3795,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4117,7 +4243,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -4544,7 +4670,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -4896,7 +5022,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -5248,7 +5374,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -5614,4 +5740,359 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
thiet ke man hinh -3
</commit_message>
<xml_diff>
--- a/03.Design/Shokai.xlsx
+++ b/03.Design/Shokai.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10065" windowHeight="4155" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Error2" sheetId="7" r:id="rId6"/>
     <sheet name="Reminder" sheetId="8" r:id="rId7"/>
     <sheet name="Registration_info" sheetId="9" r:id="rId8"/>
+    <sheet name="Mypage" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
   <si>
     <t>List item</t>
   </si>
@@ -255,7 +256,19 @@
     <t>1. Button tiếp tục sử dụng</t>
   </si>
   <si>
-    <t>1. Sau khi chạm vào mục 2 thì chuyển sang màn hình mypage</t>
+    <t>1. ImageButton sử dụng camera</t>
+  </si>
+  <si>
+    <t>2. ImageButton Edit</t>
+  </si>
+  <si>
+    <t>1. Sau khi chạm vào mục 1 thì chuyển sang màn hình mypage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Sau khi chạm vào mục 1 thì chuyển sang chế độ camera để quét ảnh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Sau khi chạm vào mục 2 thì chuyển sang màn hình Edit </t>
   </si>
 </sst>
 </file>
@@ -2759,6 +2772,189 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F417FE2A-2BCC-45FC-A2A3-67E912870960}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="257175"/>
+          <a:ext cx="3571875" cy="6353175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F63D576-9CE4-401E-A99A-9BB2D51EDE52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1495425" y="5495925"/>
+          <a:ext cx="323850" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>1</a:t>
+          </a:r>
+          <a:endParaRPr lang="vi-VN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40DAC38F-CB4B-42F9-ACC7-2B7FB8D3500E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2409825" y="5534025"/>
+          <a:ext cx="323850" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2</a:t>
+          </a:r>
+          <a:endParaRPr lang="vi-VN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4670,7 +4866,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -5022,7 +5218,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -5374,7 +5570,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -5746,8 +5942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5831,7 +6027,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="H8" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -6095,4 +6291,365 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="H8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="H9" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="H10" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
thiet ke man hinh -4
</commit_message>
<xml_diff>
--- a/03.Design/Shokai.xlsx
+++ b/03.Design/Shokai.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\03.Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6298,7 +6298,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6458,10 +6458,6 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>

</xml_diff>